<commit_message>
made the script to run off an external excel file with parameters
</commit_message>
<xml_diff>
--- a/domainParameters_example.xlsx
+++ b/domainParameters_example.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Geology\SDE_Stuff\DomainTables\PythonScripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Geology\SDE_Stuff\DomainTables\DomainScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E01AEA6F-D1D2-448D-983E-22AD9EC16EA0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FACF0C0D-D49E-4BDA-ADD9-ADB434A7DE40}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9555" windowHeight="2385" xr2:uid="{F0A731C3-9B6C-4667-9ECD-D5A3BCDB48BF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8925" activeTab="4" xr2:uid="{F0A731C3-9B6C-4667-9ECD-D5A3BCDB48BF}"/>
   </bookViews>
   <sheets>
     <sheet name="domains" sheetId="1" r:id="rId1"/>
-    <sheet name="email" sheetId="2" r:id="rId2"/>
+    <sheet name="connections" sheetId="3" r:id="rId2"/>
+    <sheet name="email" sheetId="2" r:id="rId3"/>
+    <sheet name="toAddresses" sheetId="4" r:id="rId4"/>
+    <sheet name="backup" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>password</t>
   </si>
@@ -59,13 +62,91 @@
   </si>
   <si>
     <t>DBs</t>
+  </si>
+  <si>
+    <t>PKHMapUnits</t>
+  </si>
+  <si>
+    <t>PKH list of map units</t>
+  </si>
+  <si>
+    <t>PKH_LMU$</t>
+  </si>
+  <si>
+    <t>mapunit</t>
+  </si>
+  <si>
+    <t>DomainDesc</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>HPGPS_Purpose</t>
+  </si>
+  <si>
+    <t>Purpose for HPGPS data</t>
+  </si>
+  <si>
+    <t>DomainDescrip</t>
+  </si>
+  <si>
+    <t>dbsNames</t>
+  </si>
+  <si>
+    <t>sdeConnections</t>
+  </si>
+  <si>
+    <t>Database Connections\Connection to asdfsdfsdfs_SDE.sde</t>
+  </si>
+  <si>
+    <t>Database Connections\Connection to dfsdfsdfsfdsfdfs_DBO.sde</t>
+  </si>
+  <si>
+    <t>\\sasdfafdsdsf\PKH_LMU_MASTER.xlsx</t>
+  </si>
+  <si>
+    <t>\\Idsfds\AttributeDomains_MASTER.gdb\HPGPS_Purpose</t>
+  </si>
+  <si>
+    <t>db1</t>
+  </si>
+  <si>
+    <t>db2</t>
+  </si>
+  <si>
+    <t>db3</t>
+  </si>
+  <si>
+    <t>Database Connections\Connection to asdasddfs_DBO.sde</t>
+  </si>
+  <si>
+    <t>[db1,db2,db3]</t>
+  </si>
+  <si>
+    <t>[db1]</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>sadasds@gmail.com</t>
+  </si>
+  <si>
+    <t>asdasdsa@usgs.gov</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>\\swdasdas\DomainTableBackups.gdb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +158,12 @@
       <b/>
       <sz val="9"/>
       <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -101,9 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -420,19 +510,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11AEC987-AA9D-497D-B499-5FA1301BC253}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="110.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -459,25 +551,48 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -486,6 +601,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EDD5DD-4589-4768-9506-907232768845}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907E494F-D1CF-4869-A83D-06FA1D4E1B65}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -518,4 +684,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE8EEB2B-9D4A-4718-8CFB-F10D525D3D00}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113C5616-143F-48BB-95D6-7168CE27F347}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>